<commit_message>
Updated the Gantt chart for the project
</commit_message>
<xml_diff>
--- a/Gantt project planner - RIMS MCA Group 3 .xlsx
+++ b/Gantt project planner - RIMS MCA Group 3 .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25518"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B58DF2AD-B8B8-4646-82AF-D05A8FF59F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE54789B-65B1-47CB-A14A-A35D505605CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -837,8 +837,8 @@
   </sheetPr>
   <dimension ref="B1:BO14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1"/>
@@ -1163,9 +1163,11 @@
       <c r="E7" s="12">
         <v>3</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="12">
+        <v>4</v>
+      </c>
       <c r="G7" s="13">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="44.25" customHeight="1">
@@ -1196,9 +1198,13 @@
       <c r="D9" s="12">
         <v>2</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12">
+        <v>4</v>
+      </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="2:67" ht="38.25" customHeight="1">
       <c r="B10" s="11" t="s">
@@ -1224,9 +1230,13 @@
       <c r="D11" s="12">
         <v>5</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="12">
+        <v>5</v>
+      </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1">
       <c r="B12" s="11" t="s">

</xml_diff>